<commit_message>
Adding commentary implementations for other charts.
Resolves #60.
</commit_message>
<xml_diff>
--- a/test/tracking_towards_targets.xlsx
+++ b/test/tracking_towards_targets.xlsx
@@ -5,19 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="161" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="161" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Commentary" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>tracking towards tagets</t>
   </si>
@@ -59,6 +58,30 @@
   </si>
   <si>
     <t>pesticides</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Cane and Horticulture</t>
+  </si>
+  <si>
+    <t>Grazing</t>
+  </si>
+  <si>
+    <t>Nitrogen and Pesticide</t>
+  </si>
+  <si>
+    <t>Sediment</t>
+  </si>
+  <si>
+    <t>GBR</t>
+  </si>
+  <si>
+    <t>This is the **Cane and Horticulture** commentary.</t>
+  </si>
+  <si>
+    <t>_Nothing yet._</t>
   </si>
 </sst>
 </file>
@@ -71,32 +94,32 @@
   </numFmts>
   <fonts count="5">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,10 +164,27 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+  <cellXfs count="5">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -164,13 +204,14 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="E3" activeCellId="0" pane="topLeft" sqref="E3"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3882352941176"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.7551020408163"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -347,41 +388,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.21938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="35.719387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.7551020408163"/>
   </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
-  </cols>
-  <sheetData/>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="340.25" outlineLevel="0" r="2">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>

</xml_diff>